<commit_message>
nouveau tableau de synthese
</commit_message>
<xml_diff>
--- a/projets/tableau_de_synthese.xlsx
+++ b/projets/tableau_de_synthese.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\cocojojo\projets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802663E3-A1D4-418B-818F-1E02302B0D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -18,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
-  <calcPr calcId="101716"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -101,9 +95,6 @@
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t>SESSION 2022</t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Idea-box ?</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
     <t>Adresse URL du portfolio : https://j000shua.github.io/portfolio2/</t>
   </si>
   <si>
-    <t xml:space="preserve"> Festival Sp'Or, gestion d'hebergement entre des etablissements et des equipes de sport ,application web en PHP sur le model MVC (code source, BDD, compte rendu)</t>
-  </si>
-  <si>
     <t>Parking, gestion d'attribution de place de parking, application web en PHP avec le framework Laravel (code source, BDD, MCD, documentation, maquettes, compte rendu)</t>
   </si>
   <si>
@@ -144,16 +129,41 @@
   </si>
   <si>
     <t>Centre de formation : LYC CHARLES DE FOUCAULD</t>
+  </si>
+  <si>
+    <t>Exploration d'architectures web avec Java Spring Boot, Typescript Angular et MongoDB</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Festival Sp'Or, gestion d'hebergement entre des etablissements et des equipes de sport, application web en PHP sur le model MVC (code source, BDD, compte rendu)</t>
+  </si>
+  <si>
+    <t>Projet Startup, élaboration d'un projet de startup fictive en équipe (documentation)</t>
+  </si>
+  <si>
+    <t>2021-2023</t>
+  </si>
+  <si>
+    <t>03/01/2023
+ -
+ 03/02/2023</t>
+  </si>
+  <si>
+    <t>09/05/2022
+ - 
+10/06/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -215,13 +225,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="29">
@@ -611,11 +633,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -680,15 +703,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -722,34 +769,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+  <cellStyles count="3">
+    <cellStyle name="Euro" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -769,97 +808,46 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>231540</xdr:colOff>
+      <xdr:colOff>242746</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>196080</xdr:rowOff>
+      <xdr:rowOff>274521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>350700</xdr:colOff>
+      <xdr:colOff>361906</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>358080</xdr:rowOff>
+      <xdr:rowOff>436521</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="Encre 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DFE579-86BA-6BAA-76D4-2471FFBBC5B6}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="12202560" y="1720080"/>
-            <a:ext cx="119160" cy="162000"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Encre 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DFE579-86BA-6BAA-76D4-2471FFBBC5B6}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="12193560" y="1711440"/>
-              <a:ext cx="136800" cy="179640"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Encre 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="{02DFE579-86BA-6BAA-76D4-2471FFBBC5B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11964099" y="1798521"/>
+          <a:ext cx="119160" cy="162000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-12-08T12:44:50.014"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">34 344 24575,'1'-1'0,"1"1"0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,0-3 0,22-35 0,-19 30 0,16-22 0,1 0 0,47-49 0,-57 66-227,0 0-1,-2-1 1,1-1-1,-2 1 1,11-24-1,-15 25-6598</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="911.71">331 450 24575,'-1'-7'0,"0"1"0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,0 1 0,-6-6 0,-7-8 0,-38-31 0,49 44 0,-15-11 0,2 0 0,0-1 0,1-1 0,-16-21 0,6 9 0,24 27 0,0 0 0,0 1 0,1-1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 0 0,1 1 0,0-1 0,-3-7 0,0-6-455,-1 0 0,-9-18 0,8 22-6371</inkml:trace>
-</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,7 +893,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -937,27 +925,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -989,24 +959,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1182,76 +1134,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.5546875" customWidth="1"/>
-    <col min="44" max="16384" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.5703125" customWidth="1"/>
+    <col min="44" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:43" ht="40.15" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:43" ht="40.9" customHeight="1" thickBot="1">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1">
-      <c r="A3" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:43" ht="40.15" customHeight="1">
+      <c r="A3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1">
-      <c r="A4" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+    <row r="4" spans="1:43" ht="52.5" customHeight="1">
+      <c r="A4" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1262,24 +1214,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1">
-      <c r="A5" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+    <row r="5" spans="1:43" ht="40.15" customHeight="1" thickBot="1">
+      <c r="A5" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>20</v>
+      <c r="B6" s="39" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1300,9 +1252,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.14999999999998" customHeight="1" thickBot="1">
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1357,17 +1309,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1404,18 +1356,20 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="45" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>33</v>
+      </c>
+      <c r="B9" s="44">
+        <v>44621</v>
+      </c>
       <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
-        <v>24</v>
+      <c r="D9" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>24</v>
+      <c r="F9" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
@@ -1455,22 +1409,26 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="48" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="44">
+        <v>44958</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="17"/>
+      <c r="F10" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1508,20 +1466,22 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="45.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B11" s="44">
+        <v>44896</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
-        <v>24</v>
+      <c r="F11" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
@@ -1561,15 +1521,21 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="B12" s="44">
+        <v>44986</v>
+      </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="E12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
       <c r="I12"/>
@@ -1608,7 +1574,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
       <c r="C13" s="17"/>
@@ -1653,7 +1619,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="B14" s="10"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1697,7 +1663,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="17"/>
@@ -1742,7 +1708,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A16" s="11"/>
       <c r="B16" s="10"/>
       <c r="C16" s="17"/>
@@ -1787,7 +1753,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="17"/>
@@ -1832,18 +1798,20 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="18" t="s">
-        <v>24</v>
+      <c r="H18" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -1881,17 +1849,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
-      <c r="A19" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A19" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1928,21 +1896,23 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="51.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>37</v>
+      </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="17" t="s">
-        <v>24</v>
+      <c r="D20" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="E20" s="17"/>
-      <c r="F20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>24</v>
+      <c r="F20" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20"/>
@@ -1981,7 +1951,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="17"/>
@@ -2026,7 +1996,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="10"/>
       <c r="C22" s="17"/>
@@ -2071,7 +2041,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A23" s="11"/>
       <c r="B23" s="10"/>
       <c r="C23" s="17"/>
@@ -2116,7 +2086,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="10"/>
       <c r="C24" s="17"/>
@@ -2161,7 +2131,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="17"/>
@@ -2206,7 +2176,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" s="10"/>
       <c r="C26" s="17"/>
@@ -2251,17 +2221,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
-      <c r="A27" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A27" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2298,15 +2268,21 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A28" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>36</v>
+      </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="18"/>
+      <c r="H28" s="48" t="s">
+        <v>22</v>
+      </c>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2343,7 +2319,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A29" s="11"/>
       <c r="B29" s="10"/>
       <c r="C29" s="17"/>
@@ -2388,7 +2364,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A30" s="11"/>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
@@ -2433,7 +2409,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A31" s="11"/>
       <c r="B31" s="10"/>
       <c r="C31" s="17"/>
@@ -2478,7 +2454,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A32" s="11"/>
       <c r="B32" s="10"/>
       <c r="C32" s="17"/>
@@ -2523,7 +2499,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1">
       <c r="A33" s="11"/>
       <c r="B33" s="10"/>
       <c r="C33" s="17"/>
@@ -2568,7 +2544,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" thickBot="1">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="19"/>
@@ -2613,7 +2589,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="15">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2706,11 +2682,6 @@
     <row r="81" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2718,12 +2689,17 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>